<commit_message>
Run generator for end of 2024 :stars:
</commit_message>
<xml_diff>
--- a/src/Template_Penyata_Akaun_HR_2024.xlsx
+++ b/src/Template_Penyata_Akaun_HR_2024.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="yqiVRonE0cxMGRCqODPsc2IcSnFagaR1CRu94eii4Bk="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="rH14lw611JbfZNkcDQvQm9YGEkgyS0HE53uUcNyWJzk="/>
     </ext>
   </extLst>
 </workbook>
@@ -390,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -481,6 +481,12 @@
     </xf>
     <xf borderId="21" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -1181,10 +1187,10 @@
       <c r="A38" s="4"/>
       <c r="B38" s="23"/>
       <c r="C38" s="28"/>
-      <c r="D38" s="29">
-        <v>0.0</v>
-      </c>
-      <c r="E38" s="24">
+      <c r="D38" s="37">
+        <v>0.0</v>
+      </c>
+      <c r="E38" s="38">
         <v>0.0</v>
       </c>
       <c r="F38" s="24"/>
@@ -1194,10 +1200,10 @@
       <c r="A39" s="4"/>
       <c r="B39" s="23"/>
       <c r="C39" s="28"/>
-      <c r="D39" s="29">
-        <v>0.0</v>
-      </c>
-      <c r="E39" s="24">
+      <c r="D39" s="37">
+        <v>0.0</v>
+      </c>
+      <c r="E39" s="38">
         <v>0.0</v>
       </c>
       <c r="F39" s="24"/>
@@ -1207,10 +1213,10 @@
       <c r="A40" s="4"/>
       <c r="B40" s="23"/>
       <c r="C40" s="28"/>
-      <c r="D40" s="28">
-        <v>0.0</v>
-      </c>
-      <c r="E40" s="27">
+      <c r="D40" s="29">
+        <v>0.0</v>
+      </c>
+      <c r="E40" s="24">
         <v>0.0</v>
       </c>
       <c r="F40" s="24"/>
@@ -1220,10 +1226,10 @@
       <c r="A41" s="4"/>
       <c r="B41" s="23"/>
       <c r="C41" s="28"/>
-      <c r="D41" s="28">
-        <v>0.0</v>
-      </c>
-      <c r="E41" s="27">
+      <c r="D41" s="37">
+        <v>0.0</v>
+      </c>
+      <c r="E41" s="38">
         <v>0.0</v>
       </c>
       <c r="F41" s="24"/>
@@ -1231,59 +1237,119 @@
     </row>
     <row r="42" ht="12.75" customHeight="1">
       <c r="A42" s="4"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="34">
-        <f>D34-E34+D35-E35+D36-E36+D37-E37+D38-E38+D39-E39+D41-E41+D40-E40</f>
-        <v>0</v>
-      </c>
+      <c r="B42" s="23"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="37">
+        <v>0.0</v>
+      </c>
+      <c r="E42" s="38">
+        <v>0.0</v>
+      </c>
+      <c r="F42" s="24"/>
       <c r="G42" s="6"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" ht="12.75" customHeight="1">
       <c r="A43" s="4"/>
-      <c r="B43" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="F43" s="38">
-        <f>F20+F32+F26+F42</f>
-        <v>1000</v>
-      </c>
+      <c r="B43" s="23"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="37">
+        <v>0.0</v>
+      </c>
+      <c r="E43" s="38">
+        <v>0.0</v>
+      </c>
+      <c r="F43" s="24"/>
       <c r="G43" s="6"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
       <c r="A44" s="4"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="37">
+        <v>0.0</v>
+      </c>
+      <c r="E44" s="38">
+        <v>0.0</v>
+      </c>
+      <c r="F44" s="24"/>
       <c r="G44" s="6"/>
     </row>
-    <row r="45" ht="18.75" customHeight="1">
+    <row r="45" ht="12.75" customHeight="1">
       <c r="A45" s="4"/>
-      <c r="B45" s="39" t="s">
+      <c r="B45" s="23"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="E45" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="F45" s="24"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" ht="12.75" customHeight="1">
+      <c r="A46" s="4"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="E46" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="F46" s="24"/>
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47" ht="12.75" customHeight="1">
+      <c r="A47" s="4"/>
+      <c r="B47" s="31"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="34">
+        <f>SUM(D34:D46)-SUM(E34:E46)</f>
+        <v>0</v>
+      </c>
+      <c r="G47" s="6"/>
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48" s="4"/>
+      <c r="B48" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="F48" s="40">
+        <f>SUM(F20,F26,F32,F47)</f>
+        <v>1000</v>
+      </c>
+      <c r="G48" s="6"/>
+    </row>
+    <row r="49" ht="12.75" customHeight="1">
+      <c r="A49" s="4"/>
+      <c r="G49" s="6"/>
+    </row>
+    <row r="50" ht="18.75" customHeight="1">
+      <c r="A50" s="4"/>
+      <c r="B50" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="G45" s="6"/>
-    </row>
-    <row r="46" ht="18.75" customHeight="1">
-      <c r="A46" s="4"/>
-      <c r="B46" s="39" t="s">
+      <c r="G50" s="6"/>
+    </row>
+    <row r="51" ht="18.75" customHeight="1">
+      <c r="A51" s="4"/>
+      <c r="B51" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="G46" s="6"/>
-    </row>
-    <row r="47" ht="12.75" customHeight="1">
-      <c r="A47" s="40"/>
-      <c r="B47" s="41"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="42"/>
-    </row>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
+      <c r="G51" s="6"/>
+    </row>
+    <row r="52" ht="12.75" customHeight="1">
+      <c r="A52" s="42"/>
+      <c r="B52" s="43"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="43"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="43"/>
+      <c r="G52" s="44"/>
+    </row>
     <row r="53" ht="15.75" customHeight="1"/>
     <row r="54" ht="15.75" customHeight="1"/>
     <row r="55" ht="15.75" customHeight="1"/>
@@ -2232,6 +2298,11 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="20">
     <mergeCell ref="C3:C4"/>
@@ -2243,10 +2314,10 @@
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B32:E32"/>
     <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>

</xml_diff>